<commit_message>
Update with new data for revisions
</commit_message>
<xml_diff>
--- a/Tables/01_BLtrimmer_results_comparing_MeltR_method_1_to_Meltwin_method_1/01_BLtrimmer_results_comparing_MeltR_method_1_to_Meltwin_method_1.xlsx
+++ b/Tables/01_BLtrimmer_results_comparing_MeltR_method_1_to_Meltwin_method_1/01_BLtrimmer_results_comparing_MeltR_method_1_to_Meltwin_method_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpsie\Documents\meltR.a.paper\Tables\01_BLtrimmer_results_comparing_MeltR_method_1_to_Meltwin_method_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69CEA9A3-24B3-49A3-AAFE-43A7023AD57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A04A52E6-7334-46C9-8EBB-2BC2B92EF375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="588" yWindow="948" windowWidth="13356" windowHeight="8964"/>
   </bookViews>
   <sheets>
     <sheet name="01_BLtrimmer_results_comparing_" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>Helix</t>
   </si>
@@ -64,13 +64,13 @@
     <t>ACCGGU</t>
   </si>
   <si>
-    <t>-55.03 (-57.3 to -52.39)</t>
+    <t>-54.89 (-57.11 to -51.93)</t>
   </si>
   <si>
     <t>-54.1 (Â±4)</t>
   </si>
   <si>
-    <t>-154.64 (-162 to -146.17)</t>
+    <t>-154.2 (-161.22 to -144.69)</t>
   </si>
   <si>
     <t>-151.5 (Â±12.4)</t>
@@ -82,91 +82,91 @@
     <t>-7.11 (Â±0.2)</t>
   </si>
   <si>
-    <t>45.03 (44.64 to 45.44)</t>
+    <t>45.05 (44.6 to 45.49)</t>
   </si>
   <si>
     <t>CCAUGG</t>
   </si>
   <si>
-    <t>-60.28 (-61.16 to -59.4)</t>
+    <t>-60.37 (-61.33 to -59.56)</t>
   </si>
   <si>
     <t>-60.4 (Â±2)</t>
   </si>
   <si>
-    <t>-172.47 (-175.32 to -169.73)</t>
+    <t>-172.79 (-175.85 to -170.23)</t>
   </si>
   <si>
     <t>-173.6 (Â±6.4)</t>
   </si>
   <si>
-    <t>-6.78 (-6.8 to -6.76)</t>
+    <t>-6.78 (-6.8 to -6.75)</t>
   </si>
   <si>
     <t>-6.52 (Â±0.05)</t>
   </si>
   <si>
-    <t>42.8 (42.68 to 42.88)</t>
+    <t>42.79 (42.65 to 42.88)</t>
   </si>
   <si>
     <t>CGAAAGGU/ACCUUUCG</t>
   </si>
   <si>
-    <t>-68.16 (-69.5 to -67.14)</t>
+    <t>-68.2 (-69.59 to -66.9)</t>
   </si>
   <si>
     <t>-67.02 (Â±3.025)</t>
   </si>
   <si>
-    <t>-188.27 (-192.39 to -185.14)</t>
+    <t>-188.37 (-192.64 to -184.42)</t>
   </si>
   <si>
     <t>-184.51 (Â±9.497)</t>
   </si>
   <si>
-    <t>-9.77 (-9.84 to -9.7)</t>
+    <t>-9.77 (-9.84 to -9.71)</t>
   </si>
   <si>
     <t>-9.8 (Â±0.087)</t>
   </si>
   <si>
-    <t>52.49 (52.3 to 52.69)</t>
+    <t>52.48 (52.25 to 52.64)</t>
   </si>
   <si>
     <t>CGCGCG</t>
   </si>
   <si>
-    <t>-55.78 (-57.08 to -54.69)</t>
+    <t>-55.77 (-56.62 to -55)</t>
   </si>
   <si>
     <t>-55.6 (Â±1.3)</t>
   </si>
   <si>
-    <t>-153.62 (-157.76 to -150.19)</t>
+    <t>-153.57 (-156.2 to -151.15)</t>
   </si>
   <si>
     <t>-153.9 (Â±4.3)</t>
   </si>
   <si>
-    <t>-8.14 (-8.18 to -8.1)</t>
+    <t>-8.14 (-8.18 to -8.11)</t>
   </si>
   <si>
     <t>-7.85 (Â±0.17)</t>
   </si>
   <si>
-    <t>51.32 (51.05 to 51.43)</t>
+    <t>51.34 (51.25 to 51.43)</t>
   </si>
   <si>
     <t>CGUUGC/GCAACG</t>
   </si>
   <si>
-    <t>-51.4 (-53 to -49.85)</t>
+    <t>-51.61 (-52.98 to -49.85)</t>
   </si>
   <si>
     <t>-51.06 (Â±3.567)</t>
   </si>
   <si>
-    <t>-143.12 (-148.39 to -138.13)</t>
+    <t>-143.79 (-148.21 to -138.08)</t>
   </si>
   <si>
     <t>-141.39 (Â±11.476)</t>
@@ -178,115 +178,115 @@
     <t>-7.21 (Â±0.087)</t>
   </si>
   <si>
-    <t>39.94 (39.46 to 40.29)</t>
+    <t>39.91 (39.46 to 40.3)</t>
   </si>
   <si>
     <t>CUGAGUC/GACUCAG</t>
   </si>
   <si>
-    <t>-64.29 (-65.15 to -63.34)</t>
+    <t>-64.24 (-65.12 to -63.31)</t>
   </si>
   <si>
     <t>-63.32 (Â±1.928)</t>
   </si>
   <si>
-    <t>-178 (-180.69 to -175)</t>
+    <t>-177.85 (-180.62 to -174.9)</t>
   </si>
   <si>
     <t>-174.65 (Â±6.191)</t>
   </si>
   <si>
-    <t>-9.08 (-9.11 to -9.06)</t>
+    <t>-9.08 (-9.1 to -9.06)</t>
   </si>
   <si>
     <t>-9.15 (Â±0.03)</t>
   </si>
   <si>
-    <t>49.83 (49.7 to 49.96)</t>
+    <t>49.82 (49.68 to 49.95)</t>
   </si>
   <si>
     <t>FAMCGAAAGGU/ACCUUUCGBHQ1</t>
   </si>
   <si>
-    <t>-83.74 (-87.19 to -80.92)</t>
+    <t>-83.62 (-87.32 to -79.99)</t>
   </si>
   <si>
     <t>-81.12 (Â±1.583)</t>
   </si>
   <si>
-    <t>-225.66 (-236 to -217.16)</t>
+    <t>-225.31 (-236.37 to -214.42)</t>
   </si>
   <si>
     <t>-217.61 (Â±5.076)</t>
   </si>
   <si>
-    <t>-13.76 (-13.99 to -13.57)</t>
+    <t>-13.75 (-14.01 to -13.48)</t>
   </si>
   <si>
     <t>-13.63 (Â±0.092)</t>
   </si>
   <si>
-    <t>66.28 (66.01 to 66.69)</t>
+    <t>66.28 (66.02 to 66.65)</t>
   </si>
   <si>
     <t>FAMCGUUGC/GCAACGBHQ1</t>
   </si>
   <si>
-    <t>-58.47 (-61.11 to -55.84)</t>
+    <t>-58.46 (-60.45 to -56.31)</t>
   </si>
   <si>
     <t>-61.47 (Â±3.4)</t>
   </si>
   <si>
-    <t>-155.86 (-164.09 to -147.85)</t>
+    <t>-155.88 (-161.97 to -149.38)</t>
   </si>
   <si>
     <t>-164.74 (Â±10.499)</t>
   </si>
   <si>
-    <t>-10.13 (-10.32 to -9.98)</t>
+    <t>-10.12 (-10.29 to -9.96)</t>
   </si>
   <si>
     <t>-10.38 (Â±0.163)</t>
   </si>
   <si>
-    <t>57.32 (56.83 to 58.42)</t>
+    <t>57.26 (56.88 to 58.17)</t>
   </si>
   <si>
     <t>FAMCUGAGUC/GACUCAGBHQ1</t>
   </si>
   <si>
-    <t>-75.5 (-78.58 to -73.83)</t>
+    <t>-75.26 (-77.4 to -73.85)</t>
   </si>
   <si>
     <t>-74.43 (Â±2.316)</t>
   </si>
   <si>
-    <t>-200.92 (-209.93 to -196.02)</t>
+    <t>-200.22 (-206.44 to -196.06)</t>
   </si>
   <si>
     <t>-197.46 (Â±6.709)</t>
   </si>
   <si>
-    <t>-13.19 (-13.47 to -13.04)</t>
+    <t>-13.17 (-13.4 to -13.03)</t>
   </si>
   <si>
     <t>-13.19 (Â±0.275)</t>
   </si>
   <si>
-    <t>66.98 (66.82 to 67.2)</t>
+    <t>66.99 (66.86 to 67.19)</t>
   </si>
   <si>
     <t>GAUAUAUC</t>
   </si>
   <si>
-    <t>-72.93 (-74.41 to -71.75)</t>
+    <t>-72.95 (-74.09 to -71.66)</t>
   </si>
   <si>
     <t>-74.2 (Â±4.4)</t>
   </si>
   <si>
-    <t>-217.83 (-222.65 to -214.04)</t>
+    <t>-217.88 (-221.54 to -213.71)</t>
   </si>
   <si>
     <t>-221.7 (Â±14.2)</t>
@@ -298,40 +298,61 @@
     <t>-5.41 (Â±0.06)</t>
   </si>
   <si>
-    <t>35.71 (35.57 to 35.83)</t>
+    <t>35.72 (35.58 to 35.84)</t>
   </si>
   <si>
     <t>GCAAUUGC</t>
   </si>
   <si>
-    <t>-77.58 (-78.8 to -75.79)</t>
+    <t>-77.51 (-78.71 to -75.8)</t>
   </si>
   <si>
     <t>-79.4 (Â±3.8)</t>
   </si>
   <si>
-    <t>-222.32 (-226.1 to -216.83)</t>
+    <t>-222.11 (-225.79 to -216.83)</t>
   </si>
   <si>
     <t>-229.8 (Â±11.9)</t>
   </si>
   <si>
-    <t>-8.63 (-8.68 to -8.54)</t>
+    <t>-8.63 (-8.69 to -8.55)</t>
   </si>
   <si>
     <t>-8.15 (Â±0.12)</t>
   </si>
   <si>
-    <t>49.26 (49.11 to 49.35)</t>
+    <t>49.27 (49.14 to 49.35)</t>
+  </si>
+  <si>
+    <t>UAUAUAUA</t>
+  </si>
+  <si>
+    <t>-62.24 (-66.05 to -59.75)</t>
+  </si>
+  <si>
+    <t>-63.1 (Â±2.2)</t>
+  </si>
+  <si>
+    <t>-193.76 (-206.92 to -185.22)</t>
+  </si>
+  <si>
+    <t>-196.1 (Â±7.4)</t>
+  </si>
+  <si>
+    <t>-2.14 (-2.31 to -1.87)</t>
+  </si>
+  <si>
+    <t>-2.27 (Â±0.09)</t>
+  </si>
+  <si>
+    <t>20.35 (20.08 to 20.51)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0"/>
-  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -809,9 +830,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1159,7 +1179,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1167,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="J14" sqref="J14:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1245,16 +1265,16 @@
         <v>45.4</v>
       </c>
       <c r="J2">
-        <v>1.70438926051498</v>
+        <v>1.4496742820442201</v>
       </c>
       <c r="K2">
-        <v>2.0513490559874499</v>
+        <v>1.76643768400392</v>
       </c>
       <c r="L2">
         <v>0.56417489421720801</v>
       </c>
       <c r="M2">
-        <v>0.81831250691141699</v>
+        <v>0.77390823659480701</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1286,16 +1306,16 @@
         <v>41.4</v>
       </c>
       <c r="J3">
-        <v>0.198873052701355</v>
+        <v>4.9681212221580097E-2</v>
       </c>
       <c r="K3">
-        <v>0.65304707140173701</v>
+        <v>0.467680937671412</v>
       </c>
       <c r="L3">
         <v>3.90977443609024</v>
       </c>
       <c r="M3">
-        <v>3.3254156769596199</v>
+        <v>3.3020548758760002</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1327,16 +1347,16 @@
         <v>52.9</v>
       </c>
       <c r="J4">
-        <v>1.6866400355082101</v>
+        <v>1.74530394911996</v>
       </c>
       <c r="K4">
-        <v>2.01727560491444</v>
+        <v>2.0703711649860601</v>
       </c>
       <c r="L4">
         <v>0.30659172202351698</v>
       </c>
       <c r="M4">
-        <v>0.77806243476610004</v>
+        <v>0.79711520212564402</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1368,16 +1388,16 @@
         <v>49.6</v>
       </c>
       <c r="J5">
-        <v>0.32321781289279899</v>
+        <v>0.30528867738170401</v>
       </c>
       <c r="K5">
-        <v>0.18210197710718101</v>
+        <v>0.214655088301306</v>
       </c>
       <c r="L5">
         <v>3.6272670419012001</v>
       </c>
       <c r="M5">
-        <v>3.4086405073325401</v>
+        <v>3.4475926292847299</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1409,16 +1429,16 @@
         <v>41.2</v>
       </c>
       <c r="J6">
-        <v>0.66367362873315705</v>
+        <v>1.0713937859160401</v>
       </c>
       <c r="K6">
-        <v>1.21612597096764</v>
+        <v>1.6831474857984501</v>
       </c>
       <c r="L6">
         <v>2.81293952180028</v>
       </c>
       <c r="M6">
-        <v>3.1057431599704302</v>
+        <v>3.1808654913081198</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1450,16 +1470,16 @@
         <v>50.4</v>
       </c>
       <c r="J7">
-        <v>1.52025703314788</v>
+        <v>1.44245845092505</v>
       </c>
       <c r="K7">
-        <v>1.89990075145328</v>
+        <v>1.8156028368794299</v>
       </c>
       <c r="L7">
         <v>0.76796489303346405</v>
       </c>
       <c r="M7">
-        <v>1.13738401676145</v>
+        <v>1.15745360207543</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1491,13 +1511,13 @@
         <v>66.7</v>
       </c>
       <c r="J8">
-        <v>3.1784544461967599</v>
+        <v>3.0350855894136202</v>
       </c>
       <c r="K8">
-        <v>3.6320978184853399</v>
+        <v>3.47692585568499</v>
       </c>
       <c r="L8">
-        <v>0.94925155166118302</v>
+        <v>0.87655222790357301</v>
       </c>
       <c r="M8">
         <v>0.63167393593021803</v>
@@ -1532,16 +1552,16 @@
         <v>57.7</v>
       </c>
       <c r="J9">
-        <v>5.0025012506253104</v>
+        <v>5.0195947636121003</v>
       </c>
       <c r="K9">
-        <v>5.5396132252027401</v>
+        <v>5.52679184080844</v>
       </c>
       <c r="L9">
-        <v>2.4378352023403198</v>
+        <v>2.5365853658536701</v>
       </c>
       <c r="M9">
-        <v>0.66075465136498401</v>
+        <v>0.76548364648574296</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1573,16 +1593,16 @@
         <v>67.5</v>
       </c>
       <c r="J10">
-        <v>1.42733275528579</v>
+        <v>1.10895851426281</v>
       </c>
       <c r="K10">
-        <v>1.73703499171644</v>
+        <v>1.3880506940253401</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>0.15174506828527801</v>
       </c>
       <c r="M10">
-        <v>0.77334919690659698</v>
+        <v>0.75842070042383103</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -1614,16 +1634,16 @@
         <v>35.9</v>
       </c>
       <c r="J11">
-        <v>1.7263644396112201</v>
+        <v>1.6989466530750901</v>
       </c>
       <c r="K11">
-        <v>1.76097194730734</v>
+        <v>1.73802265799172</v>
       </c>
       <c r="L11">
         <v>0.74211502782931404</v>
       </c>
       <c r="M11">
-        <v>0.53065214355536305</v>
+        <v>0.50265289025411797</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -1655,34 +1675,75 @@
         <v>47</v>
       </c>
       <c r="J12">
-        <v>2.3187667218754102</v>
+        <v>2.4090242814352201</v>
       </c>
       <c r="K12">
-        <v>3.30885605591437</v>
+        <v>3.4033325219623398</v>
       </c>
       <c r="L12">
         <v>5.7210965435041796</v>
       </c>
       <c r="M12">
-        <v>4.6956160398919602</v>
+        <v>4.7159031889477596</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="J13" s="1">
-        <f>AVERAGE(J2:J12)</f>
-        <v>1.7954973124629883</v>
-      </c>
-      <c r="K13" s="1">
-        <f t="shared" ref="K13:M13" si="0">AVERAGE(K2:K12)</f>
-        <v>2.1816704064052685</v>
-      </c>
-      <c r="L13" s="1">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G13" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" t="s">
+        <v>108</v>
+      </c>
+      <c r="I13">
+        <v>21.1</v>
+      </c>
+      <c r="J13">
+        <v>1.3722674325833699</v>
+      </c>
+      <c r="K13">
+        <v>1.2004309239214099</v>
+      </c>
+      <c r="L13">
+        <v>5.8956916099773196</v>
+      </c>
+      <c r="M13">
+        <v>3.6188178528347401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <f>AVERAGE(J2:J13)</f>
+        <v>1.7256397993325638</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ref="K14:M14" si="0">AVERAGE(K2:K13)</f>
+        <v>2.062620807669568</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="0"/>
-        <v>1.9853646213091729</v>
-      </c>
-      <c r="M13" s="1">
+        <v>2.3260415293682701</v>
+      </c>
+      <c r="M14">
         <f t="shared" si="0"/>
-        <v>1.8059640245773345</v>
+        <v>1.9709951876784286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>